<commit_message>
python search 하고 변경하기
</commit_message>
<xml_diff>
--- a/rpa_basic/1_excel/sample.xlsx
+++ b/rpa_basic/1_excel/sample.xlsx
@@ -443,7 +443,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C2" t="n">
         <v>71</v>
@@ -454,10 +454,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="C3" t="n">
-        <v>40</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4">
@@ -465,10 +465,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="C4" t="n">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5">
@@ -476,10 +476,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -487,10 +487,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="C6" t="n">
-        <v>50</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7">
@@ -498,10 +498,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>17</v>
+        <v>93</v>
       </c>
       <c r="C7" t="n">
-        <v>78</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
@@ -509,10 +509,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C8" t="n">
-        <v>5</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9">
@@ -520,10 +520,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="C9" t="n">
-        <v>86</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10">
@@ -531,10 +531,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="C10" t="n">
-        <v>74</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11">
@@ -542,10 +542,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="C11" t="n">
-        <v>43</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>